<commit_message>
added LEDs for Debugging purposes
</commit_message>
<xml_diff>
--- a/Pin Assignments.xlsx
+++ b/Pin Assignments.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cc9d343cf959b842/Documents/UT/ME 392Q Mechatronics/Final Project/bball_robot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="97" documentId="11_F25DC773A252ABDACC10489FA91E64BC5BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B21290B4-E41D-4D38-9F43-3A4B4BEB8058}"/>
+  <xr:revisionPtr revIDLastSave="101" documentId="11_F25DC773A252ABDACC10489FA91E64BC5BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F3F9A593-440C-466D-9ED9-0F13F8B8B0A7}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="32">
   <si>
     <t>Pin</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>Sensor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED </t>
   </si>
 </sst>
 </file>
@@ -322,6 +325,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -974,7 +981,7 @@
   <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1084,6 +1091,9 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
+      <c r="C10" s="6" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">

</xml_diff>

<commit_message>
updated beacon detect scripts
</commit_message>
<xml_diff>
--- a/Pin Assignments.xlsx
+++ b/Pin Assignments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cc9d343cf959b842/Documents/UT/ME 392Q Mechatronics/Final Project/bball_robot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="101" documentId="11_F25DC773A252ABDACC10489FA91E64BC5BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F3F9A593-440C-466D-9ED9-0F13F8B8B0A7}"/>
+  <xr:revisionPtr revIDLastSave="107" documentId="11_F25DC773A252ABDACC10489FA91E64BC5BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06C7707E-EAE0-4669-89B2-46BDF9BC88E5}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="33">
   <si>
     <t>Pin</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t xml:space="preserve">LED </t>
+  </si>
+  <si>
+    <t>DO NOT USE</t>
   </si>
 </sst>
 </file>
@@ -204,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -212,6 +215,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -980,8 +986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{853AEB72-36AC-4AEC-AC1C-161255D27AE9}">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1142,6 +1148,12 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -1149,7 +1161,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>30</v>
@@ -1160,12 +1172,10 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>30</v>
-      </c>
+      <c r="B17" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="7"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
@@ -1390,6 +1400,9 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B17:C17"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>